<commit_message>
v4.10 hhhhhhhhhhhhh, ask lonely_noodle for help
</commit_message>
<xml_diff>
--- a/TCM-VOTER/Data/SD.xlsx
+++ b/TCM-VOTER/Data/SD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_planting\Snoopy-Auxiliary-Code\data-washed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_planting\TCM-VOTER\TCM-VOTER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA10D1E2-7868-475C-A3C7-41E70854C5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7B2BB0-77C0-4B28-88B8-CCA9AA911C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8699,8 +8699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>